<commit_message>
doc: example description updates
</commit_message>
<xml_diff>
--- a/doc/user-guide/examples/resource/resource-alternate.xlsx
+++ b/doc/user-guide/examples/resource/resource-alternate.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\frepple\enterprise\doc\user-guide\examples\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\frepple-community\doc\user-guide\examples\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC817F9-79C3-4901-BF67-4083B28D3638}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23258" windowHeight="12578" tabRatio="813" firstSheet="3" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="sales order" sheetId="1" r:id="rId1"/>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -347,12 +346,15 @@
   </si>
   <si>
     <t>Determines whether confirmed manufacturing orders consume material or not. Default is true.</t>
+  </si>
+  <si>
+    <t>plan.webservice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
@@ -401,7 +403,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="headerstyle" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="headerstyle" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -701,21 +703,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:Q1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.53125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -823,34 +825,34 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1048576" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H1048576"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:Q1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.46484375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -933,23 +935,23 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1048576" xr:uid="{00000000-0009-0000-0000-000009000000}"/>
+  <autoFilter ref="A1:M1048576"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:M1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1026,27 +1028,27 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1048576" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>
+  <autoFilter ref="A1:E1048576"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1110,24 +1112,24 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1048576" xr:uid="{00000000-0009-0000-0000-00000B000000}"/>
+  <autoFilter ref="A1:F1048576"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="136.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="136.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1281,25 +1283,33 @@
         <v>99</v>
       </c>
     </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C1048576" xr:uid="{00000000-0009-0000-0000-00000C000000}"/>
+  <autoFilter ref="A1:C1048576"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:M1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1393,20 +1403,20 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1048576" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:E1048576"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1433,22 +1443,22 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1048576" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:B1048576"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1462,20 +1472,20 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A1048576" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <autoFilter ref="A1:A1048576"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:J1048576"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1536,7 +1546,7 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>100</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1619,22 +1629,22 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1048576" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A1:F1048576"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1648,23 +1658,23 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A1048576" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
+  <autoFilter ref="A1:A1048576"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1723,20 +1733,20 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1048576" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
+  <autoFilter ref="A1:C1048576"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1762,28 +1772,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A1048576" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
+  <autoFilter ref="A1:A1048576"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.53125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1864,7 +1874,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1048576" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
+  <autoFilter ref="A1:G1048576"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>